<commit_message>
Se agrega familia de perfiles y la tabla de perfiles canal
</commit_message>
<xml_diff>
--- a/database/Tabla_DOBLE_T.xlsx
+++ b/database/Tabla_DOBLE_T.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\Documents\cirsoc301\cirsoc301\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adiez\Documents\cirsoc301\cirsoc301\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D766777D-B8DD-4860-89B8-70126111309A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75141AF3-ACBB-425E-8040-A95802F381AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{C08AFA35-A25A-4CF1-A643-3A8FDC4FDF0E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C08AFA35-A25A-4CF1-A643-3A8FDC4FDF0E}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLA" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="360">
   <si>
     <t>d</t>
   </si>
@@ -1428,61 +1428,58 @@
     <t>4x13</t>
   </si>
   <si>
-    <t>4x117</t>
-  </si>
-  <si>
-    <t>4x102</t>
-  </si>
-  <si>
-    <t>4x89</t>
-  </si>
-  <si>
-    <t>4x73</t>
-  </si>
-  <si>
-    <t>2x84</t>
-  </si>
-  <si>
-    <t>2x74</t>
-  </si>
-  <si>
-    <t>2x63</t>
-  </si>
-  <si>
-    <t>2x53</t>
-  </si>
-  <si>
-    <t>0x57</t>
-  </si>
-  <si>
-    <t>0x42</t>
-  </si>
-  <si>
-    <t>x36</t>
-  </si>
-  <si>
-    <t>2x11.8</t>
-  </si>
-  <si>
-    <t>2x10.8</t>
-  </si>
-  <si>
-    <t>0x9</t>
-  </si>
-  <si>
-    <t>0x8</t>
-  </si>
-  <si>
-    <t>x6,5</t>
-  </si>
-  <si>
-    <t>x18,9</t>
-  </si>
-  <si>
     <t>33x241</t>
   </si>
   <si>
     <t>X2</t>
+  </si>
+  <si>
+    <t>14x117</t>
+  </si>
+  <si>
+    <t>14x102</t>
+  </si>
+  <si>
+    <t>14x89</t>
+  </si>
+  <si>
+    <t>14x73</t>
+  </si>
+  <si>
+    <t>12x84</t>
+  </si>
+  <si>
+    <t>12x74</t>
+  </si>
+  <si>
+    <t>12x63</t>
+  </si>
+  <si>
+    <t>10x57</t>
+  </si>
+  <si>
+    <t>10x42</t>
+  </si>
+  <si>
+    <t>8x36</t>
+  </si>
+  <si>
+    <t>12x11.8</t>
+  </si>
+  <si>
+    <t>12x10.8</t>
+  </si>
+  <si>
+    <t>10x9</t>
+  </si>
+  <si>
+    <t>10x8</t>
+  </si>
+  <si>
+    <t>8x6,5</t>
+  </si>
+  <si>
+    <t>5x18,9</t>
   </si>
 </sst>
 </file>
@@ -2104,9 +2101,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54AC280-589B-4A0A-9E63-8D2C52B28E53}">
   <dimension ref="A1:AF399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A369" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B400" sqref="B400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2210,7 +2207,7 @@
         <v>31</v>
       </c>
       <c r="AF1" t="s">
-        <v>360</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -16588,7 +16585,7 @@
         <v>73</v>
       </c>
       <c r="B166" t="s">
-        <v>359</v>
+        <v>342</v>
       </c>
       <c r="C166" s="7">
         <v>868</v>
@@ -33948,7 +33945,7 @@
         <v>74</v>
       </c>
       <c r="B383" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C383" s="7">
         <v>361</v>
@@ -34028,7 +34025,7 @@
         <v>74</v>
       </c>
       <c r="B384" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C384" s="7">
         <v>356</v>
@@ -34108,7 +34105,7 @@
         <v>74</v>
       </c>
       <c r="B385" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C385" s="7">
         <v>351</v>
@@ -34188,7 +34185,7 @@
         <v>74</v>
       </c>
       <c r="B386" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C386" s="7">
         <v>346</v>
@@ -34268,7 +34265,7 @@
         <v>74</v>
       </c>
       <c r="B387" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C387" s="7">
         <v>312</v>
@@ -34348,7 +34345,7 @@
         <v>74</v>
       </c>
       <c r="B388" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C388" s="7">
         <v>308</v>
@@ -34428,7 +34425,7 @@
         <v>74</v>
       </c>
       <c r="B389" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C389" s="7">
         <v>303</v>
@@ -34508,7 +34505,7 @@
         <v>74</v>
       </c>
       <c r="B390" t="s">
-        <v>349</v>
+        <v>75</v>
       </c>
       <c r="C390" s="7">
         <v>299</v>
@@ -34588,7 +34585,7 @@
         <v>74</v>
       </c>
       <c r="B391" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C391" s="7">
         <v>254</v>
@@ -34668,7 +34665,7 @@
         <v>74</v>
       </c>
       <c r="B392" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C392" s="7">
         <v>246</v>
@@ -34748,7 +34745,7 @@
         <v>74</v>
       </c>
       <c r="B393" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C393" s="7">
         <v>204</v>
@@ -34828,7 +34825,7 @@
         <v>76</v>
       </c>
       <c r="B394" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C394" s="8">
         <v>303</v>
@@ -34908,7 +34905,7 @@
         <v>76</v>
       </c>
       <c r="B395" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C395" s="8">
         <v>301</v>
@@ -34988,7 +34985,7 @@
         <v>76</v>
       </c>
       <c r="B396" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C396" s="7">
         <v>250</v>
@@ -35068,7 +35065,7 @@
         <v>76</v>
       </c>
       <c r="B397" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C397" s="7">
         <v>249</v>
@@ -35148,7 +35145,7 @@
         <v>76</v>
       </c>
       <c r="B398" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C398" s="8">
         <v>199</v>
@@ -35228,7 +35225,7 @@
         <v>76</v>
       </c>
       <c r="B399" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C399" s="9">
         <v>127</v>

</xml_diff>